<commit_message>
Se agrega código hasta angulos artirculares y funciones necesarias
</commit_message>
<xml_diff>
--- a/Integrador/TABLA ANTROPOMETRICA1.xlsx
+++ b/Integrador/TABLA ANTROPOMETRICA1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biomecanica\Documents\Registros DUPLICADO TEMPORAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Biomecánica\Biomecanica_integrador\Integrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD152578-D4A2-456E-8E51-7F7B9412EF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -299,7 +300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
@@ -676,11 +677,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1"/>
@@ -1121,6 +1122,9 @@
       <c r="AN5">
         <v>185</v>
       </c>
+      <c r="AO5">
+        <v>180</v>
+      </c>
     </row>
     <row r="6" spans="1:41">
       <c r="A6" s="3">
@@ -1214,6 +1218,9 @@
       </c>
       <c r="AN6">
         <v>79</v>
+      </c>
+      <c r="AO6">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -16753,7 +16760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16770,7 +16777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>